<commit_message>
update data settings for activate ptdf calculation
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch_bus_detailed.xlsx
+++ b/spine_rts-gmlc/datasets/branch_bus_detailed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,15 @@
     <sheet name="rel_connection__direction_node" sheetId="3" r:id="rId8"/>
     <sheet name="rel_connection__node__node" sheetId="9" r:id="rId9"/>
     <sheet name="rel_node__commodity" sheetId="5" r:id="rId10"/>
-    <sheet name="rel_node__temporal_block" sheetId="7" r:id="rId11"/>
+    <sheet name="rel_node__commodity_ptdf" sheetId="15" r:id="rId11"/>
+    <sheet name="rel_node__temporal_block" sheetId="7" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5957" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6429" uniqueCount="471">
   <si>
     <t>UID</t>
   </si>
@@ -1436,6 +1437,12 @@
   </si>
   <si>
     <t>node_opt_type_reference</t>
+  </si>
+  <si>
+    <t>energy_carrier</t>
+  </si>
+  <si>
+    <t>commodity_physics_none</t>
   </si>
 </sst>
 </file>
@@ -8088,7 +8095,7 @@
   <dimension ref="A1:E156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:XFD84"/>
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10112,6 +10119,1742 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C156"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C7" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C10" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C16" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" t="s">
+        <v>251</v>
+      </c>
+      <c r="C18" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C19" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" t="s">
+        <v>253</v>
+      </c>
+      <c r="C20" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" t="s">
+        <v>254</v>
+      </c>
+      <c r="C21" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" t="s">
+        <v>255</v>
+      </c>
+      <c r="C22" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B23" t="s">
+        <v>256</v>
+      </c>
+      <c r="C23" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>232</v>
+      </c>
+      <c r="B24" t="s">
+        <v>257</v>
+      </c>
+      <c r="C24" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>232</v>
+      </c>
+      <c r="B25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C25" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" t="s">
+        <v>259</v>
+      </c>
+      <c r="C26" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>232</v>
+      </c>
+      <c r="B27" t="s">
+        <v>260</v>
+      </c>
+      <c r="C27" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>232</v>
+      </c>
+      <c r="B28" t="s">
+        <v>261</v>
+      </c>
+      <c r="C28" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>232</v>
+      </c>
+      <c r="B29" t="s">
+        <v>262</v>
+      </c>
+      <c r="C29" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>232</v>
+      </c>
+      <c r="B30" t="s">
+        <v>263</v>
+      </c>
+      <c r="C30" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>232</v>
+      </c>
+      <c r="B31" t="s">
+        <v>264</v>
+      </c>
+      <c r="C31" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>232</v>
+      </c>
+      <c r="B32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C32" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B33" t="s">
+        <v>266</v>
+      </c>
+      <c r="C33" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>232</v>
+      </c>
+      <c r="B34" t="s">
+        <v>267</v>
+      </c>
+      <c r="C34" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" t="s">
+        <v>268</v>
+      </c>
+      <c r="C35" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>232</v>
+      </c>
+      <c r="B36" t="s">
+        <v>269</v>
+      </c>
+      <c r="C36" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>232</v>
+      </c>
+      <c r="B37" t="s">
+        <v>270</v>
+      </c>
+      <c r="C37" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>232</v>
+      </c>
+      <c r="B38" t="s">
+        <v>271</v>
+      </c>
+      <c r="C38" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>232</v>
+      </c>
+      <c r="B39" t="s">
+        <v>272</v>
+      </c>
+      <c r="C39" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>232</v>
+      </c>
+      <c r="B40" t="s">
+        <v>273</v>
+      </c>
+      <c r="C40" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>232</v>
+      </c>
+      <c r="B41" t="s">
+        <v>274</v>
+      </c>
+      <c r="C41" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>232</v>
+      </c>
+      <c r="B42" t="s">
+        <v>275</v>
+      </c>
+      <c r="C42" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>232</v>
+      </c>
+      <c r="B43" t="s">
+        <v>276</v>
+      </c>
+      <c r="C43" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>232</v>
+      </c>
+      <c r="B44" t="s">
+        <v>277</v>
+      </c>
+      <c r="C44" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>232</v>
+      </c>
+      <c r="B45" t="s">
+        <v>278</v>
+      </c>
+      <c r="C45" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" t="s">
+        <v>279</v>
+      </c>
+      <c r="C46" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>232</v>
+      </c>
+      <c r="B47" t="s">
+        <v>280</v>
+      </c>
+      <c r="C47" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>232</v>
+      </c>
+      <c r="B48" t="s">
+        <v>281</v>
+      </c>
+      <c r="C48" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>232</v>
+      </c>
+      <c r="B49" t="s">
+        <v>282</v>
+      </c>
+      <c r="C49" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>232</v>
+      </c>
+      <c r="B50" t="s">
+        <v>283</v>
+      </c>
+      <c r="C50" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>232</v>
+      </c>
+      <c r="B51" t="s">
+        <v>284</v>
+      </c>
+      <c r="C51" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>232</v>
+      </c>
+      <c r="B52" t="s">
+        <v>285</v>
+      </c>
+      <c r="C52" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>232</v>
+      </c>
+      <c r="B53" t="s">
+        <v>286</v>
+      </c>
+      <c r="C53" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>232</v>
+      </c>
+      <c r="B54" t="s">
+        <v>287</v>
+      </c>
+      <c r="C54" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>232</v>
+      </c>
+      <c r="B55" t="s">
+        <v>288</v>
+      </c>
+      <c r="C55" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>232</v>
+      </c>
+      <c r="B56" t="s">
+        <v>289</v>
+      </c>
+      <c r="C56" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>232</v>
+      </c>
+      <c r="B57" t="s">
+        <v>290</v>
+      </c>
+      <c r="C57" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>232</v>
+      </c>
+      <c r="B58" t="s">
+        <v>291</v>
+      </c>
+      <c r="C58" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" t="s">
+        <v>292</v>
+      </c>
+      <c r="C59" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" t="s">
+        <v>293</v>
+      </c>
+      <c r="C60" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>232</v>
+      </c>
+      <c r="B61" t="s">
+        <v>294</v>
+      </c>
+      <c r="C61" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>232</v>
+      </c>
+      <c r="B62" t="s">
+        <v>295</v>
+      </c>
+      <c r="C62" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>232</v>
+      </c>
+      <c r="B63" t="s">
+        <v>296</v>
+      </c>
+      <c r="C63" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>232</v>
+      </c>
+      <c r="B64" t="s">
+        <v>297</v>
+      </c>
+      <c r="C64" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>232</v>
+      </c>
+      <c r="B65" t="s">
+        <v>298</v>
+      </c>
+      <c r="C65" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>232</v>
+      </c>
+      <c r="B66" t="s">
+        <v>299</v>
+      </c>
+      <c r="C66" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>232</v>
+      </c>
+      <c r="B67" t="s">
+        <v>300</v>
+      </c>
+      <c r="C67" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>232</v>
+      </c>
+      <c r="B68" t="s">
+        <v>301</v>
+      </c>
+      <c r="C68" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>232</v>
+      </c>
+      <c r="B69" t="s">
+        <v>302</v>
+      </c>
+      <c r="C69" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>232</v>
+      </c>
+      <c r="B70" t="s">
+        <v>303</v>
+      </c>
+      <c r="C70" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>232</v>
+      </c>
+      <c r="B71" t="s">
+        <v>304</v>
+      </c>
+      <c r="C71" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>232</v>
+      </c>
+      <c r="B72" t="s">
+        <v>305</v>
+      </c>
+      <c r="C72" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>232</v>
+      </c>
+      <c r="B73" t="s">
+        <v>306</v>
+      </c>
+      <c r="C73" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>232</v>
+      </c>
+      <c r="B74" t="s">
+        <v>307</v>
+      </c>
+      <c r="C74" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>232</v>
+      </c>
+      <c r="B75" t="s">
+        <v>308</v>
+      </c>
+      <c r="C75" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>232</v>
+      </c>
+      <c r="B76" t="s">
+        <v>309</v>
+      </c>
+      <c r="C76" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>232</v>
+      </c>
+      <c r="B77" t="s">
+        <v>310</v>
+      </c>
+      <c r="C77" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>232</v>
+      </c>
+      <c r="B78" t="s">
+        <v>311</v>
+      </c>
+      <c r="C78" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>232</v>
+      </c>
+      <c r="B79" t="s">
+        <v>312</v>
+      </c>
+      <c r="C79" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>232</v>
+      </c>
+      <c r="B80" t="s">
+        <v>313</v>
+      </c>
+      <c r="C80" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>232</v>
+      </c>
+      <c r="B81" t="s">
+        <v>314</v>
+      </c>
+      <c r="C81" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>232</v>
+      </c>
+      <c r="B82" t="s">
+        <v>315</v>
+      </c>
+      <c r="C82" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>232</v>
+      </c>
+      <c r="B83" t="s">
+        <v>316</v>
+      </c>
+      <c r="C83" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>232</v>
+      </c>
+      <c r="B84" t="s">
+        <v>320</v>
+      </c>
+      <c r="C84" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>232</v>
+      </c>
+      <c r="B85" t="s">
+        <v>321</v>
+      </c>
+      <c r="C85" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>232</v>
+      </c>
+      <c r="B86" t="s">
+        <v>322</v>
+      </c>
+      <c r="C86" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>232</v>
+      </c>
+      <c r="B87" t="s">
+        <v>323</v>
+      </c>
+      <c r="C87" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>232</v>
+      </c>
+      <c r="B88" t="s">
+        <v>324</v>
+      </c>
+      <c r="C88" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>232</v>
+      </c>
+      <c r="B89" t="s">
+        <v>325</v>
+      </c>
+      <c r="C89" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>232</v>
+      </c>
+      <c r="B90" t="s">
+        <v>326</v>
+      </c>
+      <c r="C90" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>232</v>
+      </c>
+      <c r="B91" t="s">
+        <v>327</v>
+      </c>
+      <c r="C91" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>232</v>
+      </c>
+      <c r="B92" t="s">
+        <v>328</v>
+      </c>
+      <c r="C92" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>232</v>
+      </c>
+      <c r="B93" t="s">
+        <v>329</v>
+      </c>
+      <c r="C93" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>232</v>
+      </c>
+      <c r="B94" t="s">
+        <v>330</v>
+      </c>
+      <c r="C94" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>232</v>
+      </c>
+      <c r="B95" t="s">
+        <v>331</v>
+      </c>
+      <c r="C95" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>232</v>
+      </c>
+      <c r="B96" t="s">
+        <v>332</v>
+      </c>
+      <c r="C96" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>232</v>
+      </c>
+      <c r="B97" t="s">
+        <v>333</v>
+      </c>
+      <c r="C97" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>232</v>
+      </c>
+      <c r="B98" t="s">
+        <v>334</v>
+      </c>
+      <c r="C98" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>232</v>
+      </c>
+      <c r="B99" t="s">
+        <v>335</v>
+      </c>
+      <c r="C99" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>232</v>
+      </c>
+      <c r="B100" t="s">
+        <v>336</v>
+      </c>
+      <c r="C100" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>232</v>
+      </c>
+      <c r="B101" t="s">
+        <v>337</v>
+      </c>
+      <c r="C101" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>232</v>
+      </c>
+      <c r="B102" t="s">
+        <v>338</v>
+      </c>
+      <c r="C102" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>232</v>
+      </c>
+      <c r="B103" t="s">
+        <v>339</v>
+      </c>
+      <c r="C103" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>232</v>
+      </c>
+      <c r="B104" t="s">
+        <v>340</v>
+      </c>
+      <c r="C104" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>232</v>
+      </c>
+      <c r="B105" t="s">
+        <v>387</v>
+      </c>
+      <c r="C105" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>232</v>
+      </c>
+      <c r="B106" t="s">
+        <v>341</v>
+      </c>
+      <c r="C106" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>232</v>
+      </c>
+      <c r="B107" t="s">
+        <v>386</v>
+      </c>
+      <c r="C107" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>232</v>
+      </c>
+      <c r="B108" t="s">
+        <v>342</v>
+      </c>
+      <c r="C108" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>232</v>
+      </c>
+      <c r="B109" t="s">
+        <v>343</v>
+      </c>
+      <c r="C109" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>232</v>
+      </c>
+      <c r="B110" t="s">
+        <v>344</v>
+      </c>
+      <c r="C110" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>232</v>
+      </c>
+      <c r="B111" t="s">
+        <v>345</v>
+      </c>
+      <c r="C111" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>232</v>
+      </c>
+      <c r="B112" t="s">
+        <v>346</v>
+      </c>
+      <c r="C112" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>232</v>
+      </c>
+      <c r="B113" t="s">
+        <v>347</v>
+      </c>
+      <c r="C113" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>232</v>
+      </c>
+      <c r="B114" t="s">
+        <v>348</v>
+      </c>
+      <c r="C114" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>232</v>
+      </c>
+      <c r="B115" t="s">
+        <v>349</v>
+      </c>
+      <c r="C115" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>232</v>
+      </c>
+      <c r="B116" t="s">
+        <v>350</v>
+      </c>
+      <c r="C116" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" t="s">
+        <v>351</v>
+      </c>
+      <c r="C117" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>232</v>
+      </c>
+      <c r="B118" t="s">
+        <v>352</v>
+      </c>
+      <c r="C118" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>232</v>
+      </c>
+      <c r="B119" t="s">
+        <v>353</v>
+      </c>
+      <c r="C119" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>232</v>
+      </c>
+      <c r="B120" t="s">
+        <v>354</v>
+      </c>
+      <c r="C120" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>232</v>
+      </c>
+      <c r="B121" t="s">
+        <v>355</v>
+      </c>
+      <c r="C121" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>232</v>
+      </c>
+      <c r="B122" t="s">
+        <v>356</v>
+      </c>
+      <c r="C122" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>232</v>
+      </c>
+      <c r="B123" t="s">
+        <v>357</v>
+      </c>
+      <c r="C123" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>232</v>
+      </c>
+      <c r="B124" t="s">
+        <v>358</v>
+      </c>
+      <c r="C124" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>232</v>
+      </c>
+      <c r="B125" t="s">
+        <v>359</v>
+      </c>
+      <c r="C125" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>232</v>
+      </c>
+      <c r="B126" t="s">
+        <v>360</v>
+      </c>
+      <c r="C126" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>232</v>
+      </c>
+      <c r="B127" t="s">
+        <v>361</v>
+      </c>
+      <c r="C127" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>232</v>
+      </c>
+      <c r="B128" t="s">
+        <v>362</v>
+      </c>
+      <c r="C128" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>232</v>
+      </c>
+      <c r="B129" t="s">
+        <v>390</v>
+      </c>
+      <c r="C129" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>232</v>
+      </c>
+      <c r="B130" t="s">
+        <v>389</v>
+      </c>
+      <c r="C130" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>232</v>
+      </c>
+      <c r="B131" t="s">
+        <v>388</v>
+      </c>
+      <c r="C131" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>232</v>
+      </c>
+      <c r="B132" t="s">
+        <v>363</v>
+      </c>
+      <c r="C132" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>232</v>
+      </c>
+      <c r="B133" t="s">
+        <v>364</v>
+      </c>
+      <c r="C133" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>232</v>
+      </c>
+      <c r="B134" t="s">
+        <v>365</v>
+      </c>
+      <c r="C134" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>232</v>
+      </c>
+      <c r="B135" t="s">
+        <v>366</v>
+      </c>
+      <c r="C135" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>232</v>
+      </c>
+      <c r="B136" t="s">
+        <v>367</v>
+      </c>
+      <c r="C136" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>232</v>
+      </c>
+      <c r="B137" t="s">
+        <v>368</v>
+      </c>
+      <c r="C137" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>232</v>
+      </c>
+      <c r="B138" t="s">
+        <v>369</v>
+      </c>
+      <c r="C138" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>232</v>
+      </c>
+      <c r="B139" t="s">
+        <v>370</v>
+      </c>
+      <c r="C139" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>232</v>
+      </c>
+      <c r="B140" t="s">
+        <v>371</v>
+      </c>
+      <c r="C140" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>232</v>
+      </c>
+      <c r="B141" t="s">
+        <v>372</v>
+      </c>
+      <c r="C141" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>232</v>
+      </c>
+      <c r="B142" t="s">
+        <v>373</v>
+      </c>
+      <c r="C142" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>232</v>
+      </c>
+      <c r="B143" t="s">
+        <v>374</v>
+      </c>
+      <c r="C143" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>232</v>
+      </c>
+      <c r="B144" t="s">
+        <v>375</v>
+      </c>
+      <c r="C144" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>232</v>
+      </c>
+      <c r="B145" t="s">
+        <v>376</v>
+      </c>
+      <c r="C145" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>232</v>
+      </c>
+      <c r="B146" t="s">
+        <v>377</v>
+      </c>
+      <c r="C146" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>232</v>
+      </c>
+      <c r="B147" t="s">
+        <v>378</v>
+      </c>
+      <c r="C147" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>232</v>
+      </c>
+      <c r="B148" t="s">
+        <v>379</v>
+      </c>
+      <c r="C148" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>232</v>
+      </c>
+      <c r="B149" t="s">
+        <v>380</v>
+      </c>
+      <c r="C149" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>232</v>
+      </c>
+      <c r="B150" t="s">
+        <v>381</v>
+      </c>
+      <c r="C150" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>232</v>
+      </c>
+      <c r="B151" t="s">
+        <v>382</v>
+      </c>
+      <c r="C151" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>232</v>
+      </c>
+      <c r="B152" t="s">
+        <v>383</v>
+      </c>
+      <c r="C152" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>232</v>
+      </c>
+      <c r="B153" t="s">
+        <v>392</v>
+      </c>
+      <c r="C153" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>232</v>
+      </c>
+      <c r="B154" t="s">
+        <v>384</v>
+      </c>
+      <c r="C154" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>232</v>
+      </c>
+      <c r="B155" t="s">
+        <v>391</v>
+      </c>
+      <c r="C155" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>232</v>
+      </c>
+      <c r="B156" t="s">
+        <v>385</v>
+      </c>
+      <c r="C156" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C311"/>
   <sheetViews>
@@ -17440,18 +19183,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -17480,6 +19223,20 @@
       </c>
       <c r="D2" t="s">
         <v>458</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" t="s">
+        <v>469</v>
+      </c>
+      <c r="C3" t="s">
+        <v>457</v>
+      </c>
+      <c r="D3" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -20986,8 +22743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
implement piecewise heat_rate/flow_efficiency to the corresponding units
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch_bus_detailed.xlsx
+++ b/spine_rts-gmlc/datasets/branch_bus_detailed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -1468,9 +1468,6 @@
     <t>stochastic_structure</t>
   </si>
   <si>
-    <t>default_none</t>
-  </si>
-  <si>
     <t>node__stochastic_structure</t>
   </si>
   <si>
@@ -1490,6 +1487,9 @@
   </si>
   <si>
     <t>weight_relative_to_parents</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -28223,7 +28223,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28240,7 +28240,7 @@
         <v>476</v>
       </c>
       <c r="C1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D1" t="s">
         <v>462</v>
@@ -28251,16 +28251,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C2" t="s">
         <v>482</v>
       </c>
-      <c r="B2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>483</v>
-      </c>
-      <c r="D2" t="s">
-        <v>484</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -28276,7 +28276,7 @@
   <dimension ref="A1:C156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="C2:C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28299,1707 +28299,1707 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B2" t="s">
         <v>397</v>
       </c>
       <c r="C2" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B3" t="s">
         <v>236</v>
       </c>
       <c r="C3" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B4" t="s">
         <v>237</v>
       </c>
       <c r="C4" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B5" t="s">
         <v>238</v>
       </c>
       <c r="C5" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B6" t="s">
         <v>239</v>
       </c>
       <c r="C6" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B7" t="s">
         <v>240</v>
       </c>
       <c r="C7" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B8" t="s">
         <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B9" t="s">
         <v>242</v>
       </c>
       <c r="C9" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B10" t="s">
         <v>243</v>
       </c>
       <c r="C10" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B11" t="s">
         <v>244</v>
       </c>
       <c r="C11" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B12" t="s">
         <v>245</v>
       </c>
       <c r="C12" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B13" t="s">
         <v>246</v>
       </c>
       <c r="C13" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B14" t="s">
         <v>247</v>
       </c>
       <c r="C14" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B15" t="s">
         <v>248</v>
       </c>
       <c r="C15" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B16" t="s">
         <v>249</v>
       </c>
       <c r="C16" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B17" t="s">
         <v>250</v>
       </c>
       <c r="C17" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B18" t="s">
         <v>251</v>
       </c>
       <c r="C18" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B19" t="s">
         <v>252</v>
       </c>
       <c r="C19" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B20" t="s">
         <v>253</v>
       </c>
       <c r="C20" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B21" t="s">
         <v>254</v>
       </c>
       <c r="C21" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B22" t="s">
         <v>255</v>
       </c>
       <c r="C22" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B23" t="s">
         <v>256</v>
       </c>
       <c r="C23" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B24" t="s">
         <v>257</v>
       </c>
       <c r="C24" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B25" t="s">
         <v>258</v>
       </c>
       <c r="C25" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B26" t="s">
         <v>259</v>
       </c>
       <c r="C26" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B27" t="s">
         <v>260</v>
       </c>
       <c r="C27" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B28" t="s">
         <v>261</v>
       </c>
       <c r="C28" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B29" t="s">
         <v>262</v>
       </c>
       <c r="C29" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B30" t="s">
         <v>263</v>
       </c>
       <c r="C30" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B31" t="s">
         <v>264</v>
       </c>
       <c r="C31" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B32" t="s">
         <v>265</v>
       </c>
       <c r="C32" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B33" t="s">
         <v>266</v>
       </c>
       <c r="C33" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B34" t="s">
         <v>267</v>
       </c>
       <c r="C34" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B35" t="s">
         <v>268</v>
       </c>
       <c r="C35" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B36" t="s">
         <v>269</v>
       </c>
       <c r="C36" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B37" t="s">
         <v>270</v>
       </c>
       <c r="C37" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B38" t="s">
         <v>271</v>
       </c>
       <c r="C38" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B39" t="s">
         <v>272</v>
       </c>
       <c r="C39" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B40" t="s">
         <v>273</v>
       </c>
       <c r="C40" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B41" t="s">
         <v>274</v>
       </c>
       <c r="C41" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B42" t="s">
         <v>275</v>
       </c>
       <c r="C42" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B43" t="s">
         <v>276</v>
       </c>
       <c r="C43" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B44" t="s">
         <v>277</v>
       </c>
       <c r="C44" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B45" t="s">
         <v>278</v>
       </c>
       <c r="C45" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B46" t="s">
         <v>279</v>
       </c>
       <c r="C46" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B47" t="s">
         <v>280</v>
       </c>
       <c r="C47" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B48" t="s">
         <v>281</v>
       </c>
       <c r="C48" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B49" t="s">
         <v>282</v>
       </c>
       <c r="C49" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B50" t="s">
         <v>283</v>
       </c>
       <c r="C50" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B51" t="s">
         <v>284</v>
       </c>
       <c r="C51" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B52" t="s">
         <v>285</v>
       </c>
       <c r="C52" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B53" t="s">
         <v>286</v>
       </c>
       <c r="C53" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B54" t="s">
         <v>287</v>
       </c>
       <c r="C54" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B55" t="s">
         <v>288</v>
       </c>
       <c r="C55" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B56" t="s">
         <v>289</v>
       </c>
       <c r="C56" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B57" t="s">
         <v>290</v>
       </c>
       <c r="C57" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B58" t="s">
         <v>291</v>
       </c>
       <c r="C58" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B59" t="s">
         <v>292</v>
       </c>
       <c r="C59" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B60" t="s">
         <v>293</v>
       </c>
       <c r="C60" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B61" t="s">
         <v>294</v>
       </c>
       <c r="C61" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B62" t="s">
         <v>295</v>
       </c>
       <c r="C62" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B63" t="s">
         <v>296</v>
       </c>
       <c r="C63" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B64" t="s">
         <v>297</v>
       </c>
       <c r="C64" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B65" t="s">
         <v>298</v>
       </c>
       <c r="C65" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B66" t="s">
         <v>299</v>
       </c>
       <c r="C66" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B67" t="s">
         <v>300</v>
       </c>
       <c r="C67" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B68" t="s">
         <v>301</v>
       </c>
       <c r="C68" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B69" t="s">
         <v>302</v>
       </c>
       <c r="C69" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B70" t="s">
         <v>303</v>
       </c>
       <c r="C70" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B71" t="s">
         <v>304</v>
       </c>
       <c r="C71" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B72" t="s">
         <v>305</v>
       </c>
       <c r="C72" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B73" t="s">
         <v>306</v>
       </c>
       <c r="C73" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B74" t="s">
         <v>307</v>
       </c>
       <c r="C74" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B75" t="s">
         <v>308</v>
       </c>
       <c r="C75" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B76" t="s">
         <v>309</v>
       </c>
       <c r="C76" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B77" t="s">
         <v>310</v>
       </c>
       <c r="C77" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B78" t="s">
         <v>311</v>
       </c>
       <c r="C78" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B79" t="s">
         <v>312</v>
       </c>
       <c r="C79" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B80" t="s">
         <v>313</v>
       </c>
       <c r="C80" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B81" t="s">
         <v>314</v>
       </c>
       <c r="C81" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B82" t="s">
         <v>315</v>
       </c>
       <c r="C82" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B83" t="s">
         <v>316</v>
       </c>
       <c r="C83" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B84" t="s">
         <v>320</v>
       </c>
       <c r="C84" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B85" t="s">
         <v>321</v>
       </c>
       <c r="C85" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B86" t="s">
         <v>322</v>
       </c>
       <c r="C86" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B87" t="s">
         <v>323</v>
       </c>
       <c r="C87" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B88" t="s">
         <v>324</v>
       </c>
       <c r="C88" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B89" t="s">
         <v>325</v>
       </c>
       <c r="C89" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B90" t="s">
         <v>326</v>
       </c>
       <c r="C90" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B91" t="s">
         <v>327</v>
       </c>
       <c r="C91" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B92" t="s">
         <v>328</v>
       </c>
       <c r="C92" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B93" t="s">
         <v>329</v>
       </c>
       <c r="C93" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B94" t="s">
         <v>330</v>
       </c>
       <c r="C94" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B95" t="s">
         <v>331</v>
       </c>
       <c r="C95" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B96" t="s">
         <v>332</v>
       </c>
       <c r="C96" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B97" t="s">
         <v>333</v>
       </c>
       <c r="C97" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B98" t="s">
         <v>334</v>
       </c>
       <c r="C98" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B99" t="s">
         <v>335</v>
       </c>
       <c r="C99" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B100" t="s">
         <v>336</v>
       </c>
       <c r="C100" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B101" t="s">
         <v>337</v>
       </c>
       <c r="C101" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B102" t="s">
         <v>338</v>
       </c>
       <c r="C102" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B103" t="s">
         <v>339</v>
       </c>
       <c r="C103" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B104" t="s">
         <v>340</v>
       </c>
       <c r="C104" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B105" t="s">
         <v>387</v>
       </c>
       <c r="C105" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B106" t="s">
         <v>341</v>
       </c>
       <c r="C106" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B107" t="s">
         <v>386</v>
       </c>
       <c r="C107" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B108" t="s">
         <v>342</v>
       </c>
       <c r="C108" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B109" t="s">
         <v>343</v>
       </c>
       <c r="C109" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B110" t="s">
         <v>344</v>
       </c>
       <c r="C110" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B111" t="s">
         <v>345</v>
       </c>
       <c r="C111" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B112" t="s">
         <v>346</v>
       </c>
       <c r="C112" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B113" t="s">
         <v>347</v>
       </c>
       <c r="C113" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B114" t="s">
         <v>348</v>
       </c>
       <c r="C114" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B115" t="s">
         <v>349</v>
       </c>
       <c r="C115" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B116" t="s">
         <v>350</v>
       </c>
       <c r="C116" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B117" t="s">
         <v>351</v>
       </c>
       <c r="C117" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B118" t="s">
         <v>352</v>
       </c>
       <c r="C118" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B119" t="s">
         <v>353</v>
       </c>
       <c r="C119" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B120" t="s">
         <v>354</v>
       </c>
       <c r="C120" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B121" t="s">
         <v>355</v>
       </c>
       <c r="C121" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B122" t="s">
         <v>356</v>
       </c>
       <c r="C122" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B123" t="s">
         <v>357</v>
       </c>
       <c r="C123" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B124" t="s">
         <v>358</v>
       </c>
       <c r="C124" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B125" t="s">
         <v>359</v>
       </c>
       <c r="C125" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B126" t="s">
         <v>360</v>
       </c>
       <c r="C126" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B127" t="s">
         <v>361</v>
       </c>
       <c r="C127" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B128" t="s">
         <v>362</v>
       </c>
       <c r="C128" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B129" t="s">
         <v>390</v>
       </c>
       <c r="C129" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B130" t="s">
         <v>389</v>
       </c>
       <c r="C130" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B131" t="s">
         <v>388</v>
       </c>
       <c r="C131" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B132" t="s">
         <v>363</v>
       </c>
       <c r="C132" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B133" t="s">
         <v>364</v>
       </c>
       <c r="C133" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B134" t="s">
         <v>365</v>
       </c>
       <c r="C134" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B135" t="s">
         <v>366</v>
       </c>
       <c r="C135" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B136" t="s">
         <v>367</v>
       </c>
       <c r="C136" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B137" t="s">
         <v>368</v>
       </c>
       <c r="C137" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B138" t="s">
         <v>369</v>
       </c>
       <c r="C138" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B139" t="s">
         <v>370</v>
       </c>
       <c r="C139" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B140" t="s">
         <v>371</v>
       </c>
       <c r="C140" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B141" t="s">
         <v>372</v>
       </c>
       <c r="C141" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B142" t="s">
         <v>373</v>
       </c>
       <c r="C142" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B143" t="s">
         <v>374</v>
       </c>
       <c r="C143" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B144" t="s">
         <v>375</v>
       </c>
       <c r="C144" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B145" t="s">
         <v>376</v>
       </c>
       <c r="C145" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B146" t="s">
         <v>377</v>
       </c>
       <c r="C146" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B147" t="s">
         <v>378</v>
       </c>
       <c r="C147" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B148" t="s">
         <v>379</v>
       </c>
       <c r="C148" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B149" t="s">
         <v>380</v>
       </c>
       <c r="C149" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B150" t="s">
         <v>381</v>
       </c>
       <c r="C150" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B151" t="s">
         <v>382</v>
       </c>
       <c r="C151" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B152" t="s">
         <v>383</v>
       </c>
       <c r="C152" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B153" t="s">
         <v>392</v>
       </c>
       <c r="C153" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B154" t="s">
         <v>384</v>
       </c>
       <c r="C154" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B155" t="s">
         <v>391</v>
       </c>
       <c r="C155" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B156" t="s">
         <v>385</v>
       </c>
       <c r="C156" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -41886,7 +41886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C3" sqref="C3:C123"/>
     </sheetView>
   </sheetViews>
@@ -45415,8 +45415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:E76"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45434,16 +45434,16 @@
         <v>134</v>
       </c>
       <c r="B1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1" t="s">
         <v>479</v>
       </c>
-      <c r="C1" t="s">
-        <v>480</v>
-      </c>
       <c r="D1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E1" t="s">
         <v>479</v>
-      </c>
-      <c r="E1" t="s">
-        <v>480</v>
       </c>
       <c r="F1" t="s">
         <v>462</v>
@@ -47428,7 +47428,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B75" t="s">
         <v>136</v>
@@ -47440,7 +47440,7 @@
         <v>476</v>
       </c>
       <c r="E75" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update for ptdf: set `node_balance_sense` of all membering nodes of the ptdf_group to "none".
</commit_message>
<xml_diff>
--- a/spine_rts-gmlc/datasets/branch_bus_detailed.xlsx
+++ b/spine_rts-gmlc/datasets/branch_bus_detailed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="branch" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8183" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8258" uniqueCount="503">
   <si>
     <t>UID</t>
   </si>
@@ -1534,6 +1534,12 @@
   </si>
   <si>
     <t>tb2_look_ahead</t>
+  </si>
+  <si>
+    <t>nodal_balance_sense</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -8186,7 +8192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -16615,10 +16621,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16628,14 +16634,15 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>474</v>
       </c>
@@ -16648,11 +16655,14 @@
       <c r="E1" t="s">
         <v>494</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" t="s">
+        <v>494</v>
+      </c>
+      <c r="H1" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -16669,19 +16679,22 @@
         <v>464</v>
       </c>
       <c r="F2" t="s">
+        <v>501</v>
+      </c>
+      <c r="G2" t="s">
         <v>474</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>468</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>493</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>468</v>
       </c>
@@ -16696,7 +16709,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>318</v>
       </c>
@@ -16710,21 +16723,24 @@
         <v>465</v>
       </c>
       <c r="F4" t="s">
+        <v>502</v>
+      </c>
+      <c r="G4" t="s">
         <v>136</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>318</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <f>CONCATENATE("bus-",bus!A2)</f>
         <v>bus-101</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A4,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.2631578947368421E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>319</v>
       </c>
@@ -16738,21 +16754,24 @@
         <v>465</v>
       </c>
       <c r="F5" t="s">
+        <v>502</v>
+      </c>
+      <c r="G5" t="s">
         <v>136</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>319</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <f>CONCATENATE("bus-",bus!A3)</f>
         <v>bus-102</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A5,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.1345029239766082E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>320</v>
       </c>
@@ -16766,21 +16785,24 @@
         <v>465</v>
       </c>
       <c r="F6" t="s">
+        <v>502</v>
+      </c>
+      <c r="G6" t="s">
         <v>136</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>320</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" t="str">
         <f>CONCATENATE("bus-",bus!A4)</f>
         <v>bus-103</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A6,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.1052631578947368E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>321</v>
       </c>
@@ -16794,21 +16816,24 @@
         <v>465</v>
       </c>
       <c r="F7" t="s">
+        <v>502</v>
+      </c>
+      <c r="G7" t="s">
         <v>136</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>321</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" t="str">
         <f>CONCATENATE("bus-",bus!A5)</f>
         <v>bus-104</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A7,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>8.6549707602339189E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>322</v>
       </c>
@@ -16822,21 +16847,24 @@
         <v>465</v>
       </c>
       <c r="F8" t="s">
+        <v>502</v>
+      </c>
+      <c r="G8" t="s">
         <v>136</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>322</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
         <f>CONCATENATE("bus-",bus!A6)</f>
         <v>bus-105</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A8,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>8.3040935672514613E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>323</v>
       </c>
@@ -16850,21 +16878,24 @@
         <v>465</v>
       </c>
       <c r="F9" t="s">
+        <v>502</v>
+      </c>
+      <c r="G9" t="s">
         <v>136</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>323</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <f>CONCATENATE("bus-",bus!A7)</f>
         <v>bus-106</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A9,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.5906432748538011E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>324</v>
       </c>
@@ -16878,21 +16909,24 @@
         <v>465</v>
       </c>
       <c r="F10" t="s">
+        <v>502</v>
+      </c>
+      <c r="G10" t="s">
         <v>136</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>324</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" t="str">
         <f>CONCATENATE("bus-",bus!A8)</f>
         <v>bus-107</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A10,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.4619883040935672E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>325</v>
       </c>
@@ -16906,21 +16940,24 @@
         <v>465</v>
       </c>
       <c r="F11" t="s">
+        <v>502</v>
+      </c>
+      <c r="G11" t="s">
         <v>136</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>325</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" t="str">
         <f>CONCATENATE("bus-",bus!A9)</f>
         <v>bus-108</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A11,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>326</v>
       </c>
@@ -16934,21 +16971,24 @@
         <v>465</v>
       </c>
       <c r="F12" t="s">
+        <v>502</v>
+      </c>
+      <c r="G12" t="s">
         <v>136</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>326</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" t="str">
         <f>CONCATENATE("bus-",bus!A10)</f>
         <v>bus-109</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A12,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.046783625730994E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>327</v>
       </c>
@@ -16962,21 +17002,24 @@
         <v>465</v>
       </c>
       <c r="F13" t="s">
+        <v>502</v>
+      </c>
+      <c r="G13" t="s">
         <v>136</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>327</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" t="str">
         <f>CONCATENATE("bus-",bus!A11)</f>
         <v>bus-110</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A13,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.2807017543859651E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>328</v>
       </c>
@@ -16990,21 +17033,24 @@
         <v>465</v>
       </c>
       <c r="F14" t="s">
+        <v>502</v>
+      </c>
+      <c r="G14" t="s">
         <v>136</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>328</v>
       </c>
-      <c r="I14" t="str">
+      <c r="J14" t="str">
         <f>CONCATENATE("bus-",bus!A12)</f>
         <v>bus-111</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A14,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>329</v>
       </c>
@@ -17018,21 +17064,24 @@
         <v>465</v>
       </c>
       <c r="F15" t="s">
+        <v>502</v>
+      </c>
+      <c r="G15" t="s">
         <v>136</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>329</v>
       </c>
-      <c r="I15" t="str">
+      <c r="J15" t="str">
         <f>CONCATENATE("bus-",bus!A13)</f>
         <v>bus-112</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A15,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>330</v>
       </c>
@@ -17049,21 +17098,24 @@
         <v>466</v>
       </c>
       <c r="F16" t="s">
+        <v>502</v>
+      </c>
+      <c r="G16" t="s">
         <v>136</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>330</v>
       </c>
-      <c r="I16" t="str">
+      <c r="J16" t="str">
         <f>CONCATENATE("bus-",bus!A14)</f>
         <v>bus-113</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A16,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.0994152046783626E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>331</v>
       </c>
@@ -17077,21 +17129,24 @@
         <v>465</v>
       </c>
       <c r="F17" t="s">
+        <v>502</v>
+      </c>
+      <c r="G17" t="s">
         <v>136</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>331</v>
       </c>
-      <c r="I17" t="str">
+      <c r="J17" t="str">
         <f>CONCATENATE("bus-",bus!A15)</f>
         <v>bus-114</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A17,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.2690058479532163E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>332</v>
       </c>
@@ -17105,21 +17160,24 @@
         <v>465</v>
       </c>
       <c r="F18" t="s">
+        <v>502</v>
+      </c>
+      <c r="G18" t="s">
         <v>136</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>332</v>
       </c>
-      <c r="I18" t="str">
+      <c r="J18" t="str">
         <f>CONCATENATE("bus-",bus!A16)</f>
         <v>bus-115</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A18,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.7076023391812866E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>333</v>
       </c>
@@ -17133,21 +17191,24 @@
         <v>465</v>
       </c>
       <c r="F19" t="s">
+        <v>502</v>
+      </c>
+      <c r="G19" t="s">
         <v>136</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>333</v>
       </c>
-      <c r="I19" t="str">
+      <c r="J19" t="str">
         <f>CONCATENATE("bus-",bus!A17)</f>
         <v>bus-116</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A19,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.1695906432748537E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>334</v>
       </c>
@@ -17161,21 +17222,24 @@
         <v>465</v>
       </c>
       <c r="F20" t="s">
+        <v>502</v>
+      </c>
+      <c r="G20" t="s">
         <v>136</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>334</v>
       </c>
-      <c r="I20" t="str">
+      <c r="J20" t="str">
         <f>CONCATENATE("bus-",bus!A18)</f>
         <v>bus-117</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A20,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>335</v>
       </c>
@@ -17189,21 +17253,24 @@
         <v>465</v>
       </c>
       <c r="F21" t="s">
+        <v>502</v>
+      </c>
+      <c r="G21" t="s">
         <v>136</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>335</v>
       </c>
-      <c r="I21" t="str">
+      <c r="J21" t="str">
         <f>CONCATENATE("bus-",bus!A19)</f>
         <v>bus-118</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A21,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.8947368421052633E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>336</v>
       </c>
@@ -17217,21 +17284,24 @@
         <v>465</v>
       </c>
       <c r="F22" t="s">
+        <v>502</v>
+      </c>
+      <c r="G22" t="s">
         <v>136</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>336</v>
       </c>
-      <c r="I22" t="str">
+      <c r="J22" t="str">
         <f>CONCATENATE("bus-",bus!A20)</f>
         <v>bus-119</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A22,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.1169590643274852E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>337</v>
       </c>
@@ -17245,21 +17315,24 @@
         <v>465</v>
       </c>
       <c r="F23" t="s">
+        <v>502</v>
+      </c>
+      <c r="G23" t="s">
         <v>136</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>337</v>
       </c>
-      <c r="I23" t="str">
+      <c r="J23" t="str">
         <f>CONCATENATE("bus-",bus!A21)</f>
         <v>bus-120</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A23,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.4970760233918129E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>338</v>
       </c>
@@ -17273,21 +17346,24 @@
         <v>465</v>
       </c>
       <c r="F24" t="s">
+        <v>502</v>
+      </c>
+      <c r="G24" t="s">
         <v>136</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>338</v>
       </c>
-      <c r="I24" t="str">
+      <c r="J24" t="str">
         <f>CONCATENATE("bus-",bus!A22)</f>
         <v>bus-121</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A24,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>385</v>
       </c>
@@ -17301,21 +17377,24 @@
         <v>465</v>
       </c>
       <c r="F25" t="s">
+        <v>502</v>
+      </c>
+      <c r="G25" t="s">
         <v>136</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>385</v>
       </c>
-      <c r="I25" t="str">
+      <c r="J25" t="str">
         <f>CONCATENATE("bus-",bus!A23)</f>
         <v>bus-122</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A25,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>339</v>
       </c>
@@ -17329,21 +17408,24 @@
         <v>465</v>
       </c>
       <c r="F26" t="s">
+        <v>502</v>
+      </c>
+      <c r="G26" t="s">
         <v>136</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>339</v>
       </c>
-      <c r="I26" t="str">
+      <c r="J26" t="str">
         <f>CONCATENATE("bus-",bus!A24)</f>
         <v>bus-123</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A26,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>384</v>
       </c>
@@ -17357,21 +17439,24 @@
         <v>465</v>
       </c>
       <c r="F27" t="s">
+        <v>502</v>
+      </c>
+      <c r="G27" t="s">
         <v>136</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>384</v>
       </c>
-      <c r="I27" t="str">
+      <c r="J27" t="str">
         <f>CONCATENATE("bus-",bus!A25)</f>
         <v>bus-124</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A27,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>340</v>
       </c>
@@ -17385,21 +17470,24 @@
         <v>465</v>
       </c>
       <c r="F28" t="s">
+        <v>502</v>
+      </c>
+      <c r="G28" t="s">
         <v>136</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>340</v>
       </c>
-      <c r="I28" t="str">
+      <c r="J28" t="str">
         <f>CONCATENATE("bus-",bus!A26)</f>
         <v>bus-201</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A28,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.2631578947368421E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>341</v>
       </c>
@@ -17413,21 +17501,24 @@
         <v>465</v>
       </c>
       <c r="F29" t="s">
+        <v>502</v>
+      </c>
+      <c r="G29" t="s">
         <v>136</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>341</v>
       </c>
-      <c r="I29" t="str">
+      <c r="J29" t="str">
         <f>CONCATENATE("bus-",bus!A27)</f>
         <v>bus-202</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A29,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.1345029239766082E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>342</v>
       </c>
@@ -17441,21 +17532,24 @@
         <v>465</v>
       </c>
       <c r="F30" t="s">
+        <v>502</v>
+      </c>
+      <c r="G30" t="s">
         <v>136</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>342</v>
       </c>
-      <c r="I30" t="str">
+      <c r="J30" t="str">
         <f>CONCATENATE("bus-",bus!A28)</f>
         <v>bus-203</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A30,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.1052631578947368E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>343</v>
       </c>
@@ -17469,21 +17563,24 @@
         <v>465</v>
       </c>
       <c r="F31" t="s">
+        <v>502</v>
+      </c>
+      <c r="G31" t="s">
         <v>136</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>343</v>
       </c>
-      <c r="I31" t="str">
+      <c r="J31" t="str">
         <f>CONCATENATE("bus-",bus!A29)</f>
         <v>bus-204</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A31,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>8.6549707602339189E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>344</v>
       </c>
@@ -17497,21 +17594,24 @@
         <v>465</v>
       </c>
       <c r="F32" t="s">
+        <v>502</v>
+      </c>
+      <c r="G32" t="s">
         <v>136</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>344</v>
       </c>
-      <c r="I32" t="str">
+      <c r="J32" t="str">
         <f>CONCATENATE("bus-",bus!A30)</f>
         <v>bus-205</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A32,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>8.3040935672514613E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>345</v>
       </c>
@@ -17525,21 +17625,24 @@
         <v>465</v>
       </c>
       <c r="F33" t="s">
+        <v>502</v>
+      </c>
+      <c r="G33" t="s">
         <v>136</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>345</v>
       </c>
-      <c r="I33" t="str">
+      <c r="J33" t="str">
         <f>CONCATENATE("bus-",bus!A31)</f>
         <v>bus-206</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A33,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.5906432748538011E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>346</v>
       </c>
@@ -17553,21 +17656,24 @@
         <v>465</v>
       </c>
       <c r="F34" t="s">
+        <v>502</v>
+      </c>
+      <c r="G34" t="s">
         <v>136</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>346</v>
       </c>
-      <c r="I34" t="str">
+      <c r="J34" t="str">
         <f>CONCATENATE("bus-",bus!A32)</f>
         <v>bus-207</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A34,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.4619883040935672E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>347</v>
       </c>
@@ -17581,21 +17687,24 @@
         <v>465</v>
       </c>
       <c r="F35" t="s">
+        <v>502</v>
+      </c>
+      <c r="G35" t="s">
         <v>136</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>347</v>
       </c>
-      <c r="I35" t="str">
+      <c r="J35" t="str">
         <f>CONCATENATE("bus-",bus!A33)</f>
         <v>bus-208</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A35,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>348</v>
       </c>
@@ -17609,21 +17718,24 @@
         <v>465</v>
       </c>
       <c r="F36" t="s">
+        <v>502</v>
+      </c>
+      <c r="G36" t="s">
         <v>136</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>348</v>
       </c>
-      <c r="I36" t="str">
+      <c r="J36" t="str">
         <f>CONCATENATE("bus-",bus!A34)</f>
         <v>bus-209</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A36,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.046783625730994E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>349</v>
       </c>
@@ -17637,21 +17749,24 @@
         <v>465</v>
       </c>
       <c r="F37" t="s">
+        <v>502</v>
+      </c>
+      <c r="G37" t="s">
         <v>136</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>349</v>
       </c>
-      <c r="I37" t="str">
+      <c r="J37" t="str">
         <f>CONCATENATE("bus-",bus!A35)</f>
         <v>bus-210</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A37,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.2807017543859651E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>350</v>
       </c>
@@ -17665,21 +17780,24 @@
         <v>465</v>
       </c>
       <c r="F38" t="s">
+        <v>502</v>
+      </c>
+      <c r="G38" t="s">
         <v>136</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>350</v>
       </c>
-      <c r="I38" t="str">
+      <c r="J38" t="str">
         <f>CONCATENATE("bus-",bus!A36)</f>
         <v>bus-211</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A38,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>351</v>
       </c>
@@ -17693,21 +17811,24 @@
         <v>465</v>
       </c>
       <c r="F39" t="s">
+        <v>502</v>
+      </c>
+      <c r="G39" t="s">
         <v>136</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>351</v>
       </c>
-      <c r="I39" t="str">
+      <c r="J39" t="str">
         <f>CONCATENATE("bus-",bus!A37)</f>
         <v>bus-212</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A39,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>352</v>
       </c>
@@ -17721,21 +17842,24 @@
         <v>465</v>
       </c>
       <c r="F40" t="s">
+        <v>502</v>
+      </c>
+      <c r="G40" t="s">
         <v>136</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>352</v>
       </c>
-      <c r="I40" t="str">
+      <c r="J40" t="str">
         <f>CONCATENATE("bus-",bus!A38)</f>
         <v>bus-213</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A40,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.0994152046783626E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>353</v>
       </c>
@@ -17749,21 +17873,24 @@
         <v>465</v>
       </c>
       <c r="F41" t="s">
+        <v>502</v>
+      </c>
+      <c r="G41" t="s">
         <v>136</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>353</v>
       </c>
-      <c r="I41" t="str">
+      <c r="J41" t="str">
         <f>CONCATENATE("bus-",bus!A39)</f>
         <v>bus-214</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A41,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.2690058479532163E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>354</v>
       </c>
@@ -17777,21 +17904,24 @@
         <v>465</v>
       </c>
       <c r="F42" t="s">
+        <v>502</v>
+      </c>
+      <c r="G42" t="s">
         <v>136</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>354</v>
       </c>
-      <c r="I42" t="str">
+      <c r="J42" t="str">
         <f>CONCATENATE("bus-",bus!A40)</f>
         <v>bus-215</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A42,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.7076023391812866E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>355</v>
       </c>
@@ -17805,21 +17935,24 @@
         <v>465</v>
       </c>
       <c r="F43" t="s">
+        <v>502</v>
+      </c>
+      <c r="G43" t="s">
         <v>136</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>355</v>
       </c>
-      <c r="I43" t="str">
+      <c r="J43" t="str">
         <f>CONCATENATE("bus-",bus!A41)</f>
         <v>bus-216</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A43,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.1695906432748537E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>356</v>
       </c>
@@ -17833,21 +17966,24 @@
         <v>465</v>
       </c>
       <c r="F44" t="s">
+        <v>502</v>
+      </c>
+      <c r="G44" t="s">
         <v>136</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>356</v>
       </c>
-      <c r="I44" t="str">
+      <c r="J44" t="str">
         <f>CONCATENATE("bus-",bus!A42)</f>
         <v>bus-217</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A44,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>357</v>
       </c>
@@ -17861,21 +17997,24 @@
         <v>465</v>
       </c>
       <c r="F45" t="s">
+        <v>502</v>
+      </c>
+      <c r="G45" t="s">
         <v>136</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>357</v>
       </c>
-      <c r="I45" t="str">
+      <c r="J45" t="str">
         <f>CONCATENATE("bus-",bus!A43)</f>
         <v>bus-218</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A45,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.8947368421052633E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>358</v>
       </c>
@@ -17889,21 +18028,24 @@
         <v>465</v>
       </c>
       <c r="F46" t="s">
+        <v>502</v>
+      </c>
+      <c r="G46" t="s">
         <v>136</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>358</v>
       </c>
-      <c r="I46" t="str">
+      <c r="J46" t="str">
         <f>CONCATENATE("bus-",bus!A44)</f>
         <v>bus-219</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A46,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.1169590643274852E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>359</v>
       </c>
@@ -17917,21 +18059,24 @@
         <v>465</v>
       </c>
       <c r="F47" t="s">
+        <v>502</v>
+      </c>
+      <c r="G47" t="s">
         <v>136</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>359</v>
       </c>
-      <c r="I47" t="str">
+      <c r="J47" t="str">
         <f>CONCATENATE("bus-",bus!A45)</f>
         <v>bus-220</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A47,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.4970760233918129E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>360</v>
       </c>
@@ -17945,21 +18090,24 @@
         <v>465</v>
       </c>
       <c r="F48" t="s">
+        <v>502</v>
+      </c>
+      <c r="G48" t="s">
         <v>136</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>360</v>
       </c>
-      <c r="I48" t="str">
+      <c r="J48" t="str">
         <f>CONCATENATE("bus-",bus!A46)</f>
         <v>bus-221</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A48,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>388</v>
       </c>
@@ -17973,21 +18121,24 @@
         <v>465</v>
       </c>
       <c r="F49" t="s">
+        <v>502</v>
+      </c>
+      <c r="G49" t="s">
         <v>136</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>388</v>
       </c>
-      <c r="I49" t="str">
+      <c r="J49" t="str">
         <f>CONCATENATE("bus-",bus!A47)</f>
         <v>bus-222</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A49,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>387</v>
       </c>
@@ -18001,21 +18152,24 @@
         <v>465</v>
       </c>
       <c r="F50" t="s">
+        <v>502</v>
+      </c>
+      <c r="G50" t="s">
         <v>136</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>387</v>
       </c>
-      <c r="I50" t="str">
+      <c r="J50" t="str">
         <f>CONCATENATE("bus-",bus!A48)</f>
         <v>bus-223</v>
       </c>
-      <c r="J50">
+      <c r="K50">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A50,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>386</v>
       </c>
@@ -18029,21 +18183,24 @@
         <v>465</v>
       </c>
       <c r="F51" t="s">
+        <v>502</v>
+      </c>
+      <c r="G51" t="s">
         <v>136</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>386</v>
       </c>
-      <c r="I51" t="str">
+      <c r="J51" t="str">
         <f>CONCATENATE("bus-",bus!A49)</f>
         <v>bus-224</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A51,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>361</v>
       </c>
@@ -18057,21 +18214,24 @@
         <v>465</v>
       </c>
       <c r="F52" t="s">
+        <v>502</v>
+      </c>
+      <c r="G52" t="s">
         <v>136</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>361</v>
       </c>
-      <c r="I52" t="str">
+      <c r="J52" t="str">
         <f>CONCATENATE("bus-",bus!A50)</f>
         <v>bus-301</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A52,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.2631578947368421E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>362</v>
       </c>
@@ -18085,21 +18245,24 @@
         <v>465</v>
       </c>
       <c r="F53" t="s">
+        <v>502</v>
+      </c>
+      <c r="G53" t="s">
         <v>136</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>362</v>
       </c>
-      <c r="I53" t="str">
+      <c r="J53" t="str">
         <f>CONCATENATE("bus-",bus!A51)</f>
         <v>bus-302</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A53,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.1345029239766082E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>363</v>
       </c>
@@ -18113,21 +18276,24 @@
         <v>465</v>
       </c>
       <c r="F54" t="s">
+        <v>502</v>
+      </c>
+      <c r="G54" t="s">
         <v>136</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>363</v>
       </c>
-      <c r="I54" t="str">
+      <c r="J54" t="str">
         <f>CONCATENATE("bus-",bus!A52)</f>
         <v>bus-303</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A54,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.1052631578947368E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>364</v>
       </c>
@@ -18141,21 +18307,24 @@
         <v>465</v>
       </c>
       <c r="F55" t="s">
+        <v>502</v>
+      </c>
+      <c r="G55" t="s">
         <v>136</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>364</v>
       </c>
-      <c r="I55" t="str">
+      <c r="J55" t="str">
         <f>CONCATENATE("bus-",bus!A53)</f>
         <v>bus-304</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A55,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>8.6549707602339189E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>365</v>
       </c>
@@ -18169,21 +18338,24 @@
         <v>465</v>
       </c>
       <c r="F56" t="s">
+        <v>502</v>
+      </c>
+      <c r="G56" t="s">
         <v>136</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>365</v>
       </c>
-      <c r="I56" t="str">
+      <c r="J56" t="str">
         <f>CONCATENATE("bus-",bus!A54)</f>
         <v>bus-305</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A56,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>8.3040935672514613E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>366</v>
       </c>
@@ -18197,21 +18369,24 @@
         <v>465</v>
       </c>
       <c r="F57" t="s">
+        <v>502</v>
+      </c>
+      <c r="G57" t="s">
         <v>136</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>366</v>
       </c>
-      <c r="I57" t="str">
+      <c r="J57" t="str">
         <f>CONCATENATE("bus-",bus!A55)</f>
         <v>bus-306</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A57,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.5906432748538011E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>367</v>
       </c>
@@ -18225,21 +18400,24 @@
         <v>465</v>
       </c>
       <c r="F58" t="s">
+        <v>502</v>
+      </c>
+      <c r="G58" t="s">
         <v>136</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>367</v>
       </c>
-      <c r="I58" t="str">
+      <c r="J58" t="str">
         <f>CONCATENATE("bus-",bus!A56)</f>
         <v>bus-307</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A58,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.4619883040935672E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>368</v>
       </c>
@@ -18253,21 +18431,24 @@
         <v>465</v>
       </c>
       <c r="F59" t="s">
+        <v>502</v>
+      </c>
+      <c r="G59" t="s">
         <v>136</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>368</v>
       </c>
-      <c r="I59" t="str">
+      <c r="J59" t="str">
         <f>CONCATENATE("bus-",bus!A57)</f>
         <v>bus-308</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A59,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0.02</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>369</v>
       </c>
@@ -18281,21 +18462,24 @@
         <v>465</v>
       </c>
       <c r="F60" t="s">
+        <v>502</v>
+      </c>
+      <c r="G60" t="s">
         <v>136</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>369</v>
       </c>
-      <c r="I60" t="str">
+      <c r="J60" t="str">
         <f>CONCATENATE("bus-",bus!A58)</f>
         <v>bus-309</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A60,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.046783625730994E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>370</v>
       </c>
@@ -18309,21 +18493,24 @@
         <v>465</v>
       </c>
       <c r="F61" t="s">
+        <v>502</v>
+      </c>
+      <c r="G61" t="s">
         <v>136</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>370</v>
       </c>
-      <c r="I61" t="str">
+      <c r="J61" t="str">
         <f>CONCATENATE("bus-",bus!A59)</f>
         <v>bus-310</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A61,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.2807017543859651E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>371</v>
       </c>
@@ -18337,21 +18524,24 @@
         <v>465</v>
       </c>
       <c r="F62" t="s">
+        <v>502</v>
+      </c>
+      <c r="G62" t="s">
         <v>136</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>371</v>
       </c>
-      <c r="I62" t="str">
+      <c r="J62" t="str">
         <f>CONCATENATE("bus-",bus!A60)</f>
         <v>bus-311</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A62,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>372</v>
       </c>
@@ -18365,21 +18555,24 @@
         <v>465</v>
       </c>
       <c r="F63" t="s">
+        <v>502</v>
+      </c>
+      <c r="G63" t="s">
         <v>136</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>372</v>
       </c>
-      <c r="I63" t="str">
+      <c r="J63" t="str">
         <f>CONCATENATE("bus-",bus!A61)</f>
         <v>bus-312</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A63,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>373</v>
       </c>
@@ -18393,21 +18586,24 @@
         <v>465</v>
       </c>
       <c r="F64" t="s">
+        <v>502</v>
+      </c>
+      <c r="G64" t="s">
         <v>136</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>373</v>
       </c>
-      <c r="I64" t="str">
+      <c r="J64" t="str">
         <f>CONCATENATE("bus-",bus!A62)</f>
         <v>bus-313</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A64,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.0994152046783626E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>374</v>
       </c>
@@ -18421,21 +18617,24 @@
         <v>465</v>
       </c>
       <c r="F65" t="s">
+        <v>502</v>
+      </c>
+      <c r="G65" t="s">
         <v>136</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>374</v>
       </c>
-      <c r="I65" t="str">
+      <c r="J65" t="str">
         <f>CONCATENATE("bus-",bus!A63)</f>
         <v>bus-314</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A65,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.2690058479532163E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>375</v>
       </c>
@@ -18449,21 +18648,24 @@
         <v>465</v>
       </c>
       <c r="F66" t="s">
+        <v>502</v>
+      </c>
+      <c r="G66" t="s">
         <v>136</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>375</v>
       </c>
-      <c r="I66" t="str">
+      <c r="J66" t="str">
         <f>CONCATENATE("bus-",bus!A64)</f>
         <v>bus-315</v>
       </c>
-      <c r="J66">
+      <c r="K66">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A66,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.7076023391812866E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>376</v>
       </c>
@@ -18477,21 +18679,24 @@
         <v>465</v>
       </c>
       <c r="F67" t="s">
+        <v>502</v>
+      </c>
+      <c r="G67" t="s">
         <v>136</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>376</v>
       </c>
-      <c r="I67" t="str">
+      <c r="J67" t="str">
         <f>CONCATENATE("bus-",bus!A65)</f>
         <v>bus-316</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A67,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.1695906432748537E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>377</v>
       </c>
@@ -18505,21 +18710,24 @@
         <v>465</v>
       </c>
       <c r="F68" t="s">
+        <v>502</v>
+      </c>
+      <c r="G68" t="s">
         <v>136</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>377</v>
       </c>
-      <c r="I68" t="str">
+      <c r="J68" t="str">
         <f>CONCATENATE("bus-",bus!A66)</f>
         <v>bus-317</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A68,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>378</v>
       </c>
@@ -18533,21 +18741,24 @@
         <v>465</v>
       </c>
       <c r="F69" t="s">
+        <v>502</v>
+      </c>
+      <c r="G69" t="s">
         <v>136</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>378</v>
       </c>
-      <c r="I69" t="str">
+      <c r="J69" t="str">
         <f>CONCATENATE("bus-",bus!A67)</f>
         <v>bus-318</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A69,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>3.8947368421052633E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>379</v>
       </c>
@@ -18561,21 +18772,24 @@
         <v>465</v>
       </c>
       <c r="F70" t="s">
+        <v>502</v>
+      </c>
+      <c r="G70" t="s">
         <v>136</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>379</v>
       </c>
-      <c r="I70" t="str">
+      <c r="J70" t="str">
         <f>CONCATENATE("bus-",bus!A68)</f>
         <v>bus-319</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A70,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>2.1169590643274852E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>380</v>
       </c>
@@ -18589,21 +18803,24 @@
         <v>465</v>
       </c>
       <c r="F71" t="s">
+        <v>502</v>
+      </c>
+      <c r="G71" t="s">
         <v>136</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>380</v>
       </c>
-      <c r="I71" t="str">
+      <c r="J71" t="str">
         <f>CONCATENATE("bus-",bus!A69)</f>
         <v>bus-320</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A71,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>1.4970760233918129E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>381</v>
       </c>
@@ -18617,21 +18834,24 @@
         <v>465</v>
       </c>
       <c r="F72" t="s">
+        <v>502</v>
+      </c>
+      <c r="G72" t="s">
         <v>136</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>381</v>
       </c>
-      <c r="I72" t="str">
+      <c r="J72" t="str">
         <f>CONCATENATE("bus-",bus!A70)</f>
         <v>bus-321</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A72,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>390</v>
       </c>
@@ -18645,21 +18865,24 @@
         <v>465</v>
       </c>
       <c r="F73" t="s">
+        <v>502</v>
+      </c>
+      <c r="G73" t="s">
         <v>136</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>390</v>
       </c>
-      <c r="I73" t="str">
+      <c r="J73" t="str">
         <f>CONCATENATE("bus-",bus!A71)</f>
         <v>bus-322</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A73,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>382</v>
       </c>
@@ -18673,21 +18896,24 @@
         <v>465</v>
       </c>
       <c r="F74" t="s">
+        <v>502</v>
+      </c>
+      <c r="G74" t="s">
         <v>136</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>382</v>
       </c>
-      <c r="I74" t="str">
+      <c r="J74" t="str">
         <f>CONCATENATE("bus-",bus!A72)</f>
         <v>bus-323</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A74,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>389</v>
       </c>
@@ -18701,21 +18927,24 @@
         <v>465</v>
       </c>
       <c r="F75" t="s">
+        <v>502</v>
+      </c>
+      <c r="G75" t="s">
         <v>136</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>389</v>
       </c>
-      <c r="I75" t="str">
+      <c r="J75" t="str">
         <f>CONCATENATE("bus-",bus!A73)</f>
         <v>bus-324</v>
       </c>
-      <c r="J75">
+      <c r="K75">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A75,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>383</v>
       </c>
@@ -18729,16 +18958,19 @@
         <v>465</v>
       </c>
       <c r="F76" t="s">
+        <v>502</v>
+      </c>
+      <c r="G76" t="s">
         <v>136</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>383</v>
       </c>
-      <c r="I76" t="str">
+      <c r="J76" t="str">
         <f>CONCATENATE("bus-",bus!A74)</f>
         <v>bus-325</v>
       </c>
-      <c r="J76">
+      <c r="K76">
         <f>VLOOKUP(_xlfn.NUMBERVALUE(RIGHT(A76,3)),bus!$A$2:$E$74,5,FALSE)/SUM(bus!$E$2:$E$74)</f>
         <v>0</v>
       </c>

</xml_diff>